<commit_message>
Agrego funcionalidad de reporte de clientes
</commit_message>
<xml_diff>
--- a/reporte_ventas_2.xlsx
+++ b/reporte_ventas_2.xlsx
@@ -11,7 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Medio de Venta" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Detalle Ventas'!$A$1:$J$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Detalle Ventas'!$A$1:$J$24</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1236,38 +1236,266 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="inlineStr"/>
-      <c r="B19" s="3" t="inlineStr"/>
-      <c r="C19" s="3" t="inlineStr"/>
-      <c r="D19" s="3" t="inlineStr"/>
-      <c r="E19" s="3" t="inlineStr">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G19" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G20" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>8</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G21" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>9</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G22" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>9</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G23" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Torta Argenta (Entera)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>27-02-2025</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>22936.83</v>
+      </c>
+      <c r="G24" t="n">
+        <v>47400</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>24463.17</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>1.066545377020277</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr"/>
+      <c r="B25" s="3" t="inlineStr"/>
+      <c r="C25" s="3" t="inlineStr"/>
+      <c r="D25" s="3" t="inlineStr"/>
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="F19" s="3">
-        <f>SUBTOTAL(9,F2:F18)</f>
+      <c r="F25" s="3">
+        <f>SUBTOTAL(9,F2:F24)</f>
         <v/>
       </c>
-      <c r="G19" s="3">
-        <f>SUBTOTAL(9,G2:G18)</f>
+      <c r="G25" s="3">
+        <f>SUBTOTAL(9,G2:G24)</f>
         <v/>
       </c>
-      <c r="H19" s="3">
-        <f>SUBTOTAL(9,H2:H18)</f>
+      <c r="H25" s="3">
+        <f>SUBTOTAL(9,H2:H24)</f>
         <v/>
       </c>
-      <c r="I19" s="3">
-        <f>SUBTOTAL(9,I2:I18)</f>
+      <c r="I25" s="3">
+        <f>SUBTOTAL(9,I2:I24)</f>
         <v/>
       </c>
-      <c r="J19" s="4">
-        <f>I19/F19</f>
+      <c r="J25" s="4">
+        <f>I25/F25</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J18"/>
+  <autoFilter ref="A1:J24"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1315,7 +1543,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -1325,7 +1553,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>